<commit_message>
menambahkan custom datatable menambahkan edit password menambahkan filter untuk detail simpanan berdasar range waktu, tahun, bulan menambahkan tambah pengguna
</commit_message>
<xml_diff>
--- a/excel/import_data.xlsx
+++ b/excel/import_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andika\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116A177A-EED2-4740-905A-BB27BA3FD0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288F5E28-C599-4718-B16B-6212757D5B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>NAMA</t>
   </si>
@@ -36,13 +36,16 @@
     <t>NIK</t>
   </si>
   <si>
-    <t>NO HP</t>
-  </si>
-  <si>
-    <t>Anduika</t>
-  </si>
-  <si>
-    <t>ggrgr</t>
+    <t>JENIS KELAMIN</t>
+  </si>
+  <si>
+    <t>Puput</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
+  </si>
+  <si>
+    <t>Pengkok</t>
   </si>
 </sst>
 </file>
@@ -383,15 +386,15 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1234</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -399,8 +402,8 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>7867677</v>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>